<commit_message>
child income bugfix, ALG2 test extended
Former-commit-id: cf9e455ee7236933a3fac4d6ac11fad7254bb19e
</commit_message>
<xml_diff>
--- a/pre-waf/tests/test_data/test_dfs_alg2.xlsx
+++ b/pre-waf/tests/test_data/test_dfs_alg2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>hid</t>
   </si>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV29"/>
+  <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,12 +553,11 @@
     <col min="34" max="34" width="15.7109375" customWidth="1"/>
     <col min="38" max="38" width="12.5703125" customWidth="1"/>
     <col min="39" max="39" width="14.7109375" customWidth="1"/>
-    <col min="40" max="40" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="16.140625" customWidth="1"/>
-    <col min="42" max="42" width="9.28515625" customWidth="1"/>
+    <col min="40" max="40" width="16.140625" customWidth="1"/>
+    <col min="41" max="41" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -676,21 +675,18 @@
       <c r="AM1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AN1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="14" t="s">
-        <v>32</v>
+      <c r="AO1" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="AP1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="13"/>
+      <c r="AQ1" s="13"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -714,7 +710,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H16" si="0">AG2-G2</f>
+        <f t="shared" ref="H2:H19" si="0">AG2-G2</f>
         <v>1986</v>
       </c>
       <c r="I2">
@@ -804,7 +800,7 @@
         <v>460</v>
       </c>
       <c r="AJ2" s="26">
-        <f>$AP2-$AQ2</f>
+        <f>$AO2-$AP2</f>
         <v>400</v>
       </c>
       <c r="AK2">
@@ -818,24 +814,23 @@
         <f t="shared" ref="AM2:AM14" si="2">I2+J2</f>
         <v>800</v>
       </c>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="26">
+      <c r="AN2" s="26">
         <f>AL2+AM2</f>
         <v>1765</v>
       </c>
-      <c r="AP2" s="11">
+      <c r="AO2" s="11">
         <f>U2-AB2-AC2-AD2</f>
         <v>680</v>
       </c>
-      <c r="AQ2">
+      <c r="AP2">
         <f>100+0.2*(U2-100)</f>
         <v>280</v>
       </c>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="5"/>
-      <c r="AV2" s="11"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="5"/>
+      <c r="AU2" s="11"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -949,7 +944,7 @@
         <v>460</v>
       </c>
       <c r="AJ3" s="1">
-        <f t="shared" ref="AJ3:AJ16" si="7">$AP3-$AQ3</f>
+        <f t="shared" ref="AJ3:AJ19" si="7">$AO3-$AP3</f>
         <v>0</v>
       </c>
       <c r="AK3">
@@ -963,23 +958,22 @@
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="26">
-        <f t="shared" ref="AO3:AO16" si="9">AL3+AM3</f>
+      <c r="AN3" s="26">
+        <f t="shared" ref="AN3:AN16" si="9">AL3+AM3</f>
         <v>1765</v>
       </c>
-      <c r="AP3" s="11">
+      <c r="AO3" s="11">
         <f>U3-AB3-AC3-AD3</f>
         <v>0</v>
       </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="9"/>
-      <c r="AS3" s="5"/>
-      <c r="AV3" s="11"/>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="5"/>
+      <c r="AU3" s="11"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1107,22 +1101,21 @@
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="26">
+      <c r="AN4" s="26">
         <f t="shared" si="9"/>
         <v>1765</v>
       </c>
-      <c r="AP4" s="11">
+      <c r="AO4" s="11">
         <v>160</v>
       </c>
-      <c r="AQ4">
+      <c r="AP4">
         <v>100</v>
       </c>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="5"/>
-      <c r="AV4" s="11"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="5"/>
+      <c r="AU4" s="11"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1249,26 +1242,25 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="27">
+      <c r="AN5" s="27">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
-      <c r="AP5" s="15">
+      <c r="AO5" s="15">
         <f>U5+Y5-AB5-AC5-AD5</f>
         <v>740</v>
       </c>
-      <c r="AQ5">
+      <c r="AP5">
         <f>100+0.2*(U5-100)</f>
         <v>240</v>
       </c>
-      <c r="AR5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="8"/>
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="11"/>
+      <c r="AU5" s="11"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1395,25 +1387,24 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="28">
+      <c r="AN6" s="28">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
-      <c r="AP6" s="19">
-        <f t="shared" ref="AP5:AP16" si="10">U6-AB6-AC6-AD6</f>
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="20"/>
+      <c r="AO6" s="19">
+        <f t="shared" ref="AO6:AO16" si="10">U6-AB6-AC6-AD6</f>
+        <v>0</v>
+      </c>
+      <c r="AP6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="6"/>
       <c r="AS6" s="6"/>
       <c r="AT6" s="6"/>
-      <c r="AU6" s="6"/>
-      <c r="AV6" s="11"/>
+      <c r="AU6" s="11"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1541,26 +1532,25 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN7" s="9"/>
-      <c r="AO7" s="27">
+      <c r="AN7" s="27">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
-      <c r="AP7" s="15">
+      <c r="AO7" s="15">
         <f>U7+Y7-AB7-AC7-AD7</f>
         <v>944.5</v>
       </c>
-      <c r="AQ7">
+      <c r="AP7">
         <f>100+0.2*(700)+0.1*200</f>
         <v>260</v>
       </c>
-      <c r="AR7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="8"/>
       <c r="AS7" s="8"/>
       <c r="AT7" s="8"/>
-      <c r="AU7" s="8"/>
-      <c r="AV7" s="15"/>
+      <c r="AU7" s="15"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1688,25 +1678,24 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="29">
+      <c r="AN8" s="29">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
-      <c r="AP8" s="17">
+      <c r="AO8" s="17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="9"/>
+      <c r="AP8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
       <c r="AT8" s="3"/>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="17"/>
+      <c r="AU8" s="17"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1834,25 +1823,24 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="27">
+      <c r="AN9" s="27">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AP9" s="15">
+      <c r="AO9" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="16"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="11"/>
+      <c r="AP9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="10"/>
+      <c r="AR9" s="16"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="11"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1980,25 +1968,24 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="29">
+      <c r="AN10" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AP10" s="17">
+      <c r="AO10" s="17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="18"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="4"/>
-      <c r="AV10" s="11"/>
+      <c r="AP10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="18"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="11"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2126,24 +2113,23 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN11" s="9"/>
-      <c r="AO11" s="29">
+      <c r="AN11" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AP11" s="11">
+      <c r="AO11" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="9"/>
-      <c r="AS11" s="5"/>
-      <c r="AT11" s="3"/>
-      <c r="AV11" s="11"/>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="3"/>
+      <c r="AU11" s="11"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2271,24 +2257,23 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="29">
+      <c r="AN12" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AP12" s="11">
+      <c r="AO12" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ12">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="5"/>
-      <c r="AT12" s="3"/>
-      <c r="AV12" s="11"/>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="3"/>
+      <c r="AU12" s="11"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2416,24 +2401,23 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="29">
+      <c r="AN13" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AP13" s="11">
+      <c r="AO13" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="9"/>
-      <c r="AS13" s="5"/>
-      <c r="AT13" s="3"/>
-      <c r="AV13" s="11"/>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="3"/>
+      <c r="AU13" s="11"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2552,29 +2536,28 @@
         <v>0</v>
       </c>
       <c r="AL14" s="8">
-        <f>291*3</f>
-        <v>873</v>
+        <f>2*328+291</f>
+        <v>947</v>
       </c>
       <c r="AM14" s="2">
         <f t="shared" si="2"/>
         <v>830</v>
       </c>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="27">
+      <c r="AN14" s="27">
         <f t="shared" si="9"/>
-        <v>1703</v>
-      </c>
-      <c r="AP14" s="2">
+        <v>1777</v>
+      </c>
+      <c r="AO14" s="2">
         <f t="shared" si="10"/>
         <v>1149</v>
       </c>
-      <c r="AQ14">
+      <c r="AP14">
         <f>100+0.2*900+0.1*200</f>
         <v>300</v>
       </c>
-      <c r="AR14" s="9"/>
+      <c r="AQ14" s="9"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -2690,28 +2673,28 @@
       <c r="AK15" s="3">
         <v>0</v>
       </c>
-      <c r="AL15">
-        <f t="shared" ref="AL15:AL16" si="14">291*3</f>
-        <v>873</v>
+      <c r="AL15" s="8">
+        <f>2*328+291</f>
+        <v>947</v>
       </c>
       <c r="AM15">
-        <f t="shared" ref="AM15:AM16" si="15">I15+J15</f>
+        <f t="shared" ref="AM15:AM16" si="14">I15+J15</f>
         <v>830</v>
       </c>
-      <c r="AO15" s="26">
+      <c r="AN15" s="26">
         <f t="shared" si="9"/>
-        <v>1703</v>
+        <v>1777</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="AP15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="9"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -2827,88 +2810,482 @@
       <c r="AK16" s="3">
         <v>0</v>
       </c>
-      <c r="AL16">
+      <c r="AL16" s="8">
+        <f>2*328+291</f>
+        <v>947</v>
+      </c>
+      <c r="AM16">
         <f t="shared" si="14"/>
-        <v>873</v>
-      </c>
-      <c r="AM16">
-        <f t="shared" si="15"/>
         <v>830</v>
       </c>
-      <c r="AO16" s="26">
+      <c r="AN16" s="26">
         <f t="shared" si="9"/>
-        <v>1703</v>
-      </c>
-      <c r="AP16">
+        <v>1777</v>
+      </c>
+      <c r="AO16">
         <f t="shared" si="10"/>
         <v>680</v>
       </c>
-      <c r="AQ16">
+      <c r="AP16">
         <f>100+0.2*(U16-100)</f>
         <v>240</v>
       </c>
-      <c r="AR16" s="9"/>
+      <c r="AQ16" s="9"/>
     </row>
-    <row r="17" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="25"/>
-      <c r="AO17" s="9"/>
-      <c r="AR17" s="9"/>
+    <row r="17" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1989</v>
+      </c>
+      <c r="I17" s="2">
+        <v>438</v>
+      </c>
+      <c r="J17" s="2">
+        <v>80</v>
+      </c>
+      <c r="K17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>2</v>
+      </c>
+      <c r="P17" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1</v>
+      </c>
+      <c r="S17" s="2">
+        <v>1</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>800</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="2">
+        <f>0.17*U17</f>
+        <v>136</v>
+      </c>
+      <c r="AE17" s="2">
+        <f>2*194</f>
+        <v>388</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>2019</v>
+      </c>
+      <c r="AH17" s="1">
+        <f>AI17+AE17</f>
+        <v>812</v>
+      </c>
+      <c r="AI17" s="21">
+        <f>AJ17+AJ19</f>
+        <v>424</v>
+      </c>
+      <c r="AJ17" s="1">
+        <f t="shared" si="7"/>
+        <v>424</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="AL17">
+        <f>(1+AK17)*424+(245+302)</f>
+        <v>1123.6399999999999</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" ref="AM17:AM19" si="15">I17+J17</f>
+        <v>518</v>
+      </c>
+      <c r="AN17" s="26">
+        <f>AL17+AM17</f>
+        <v>1641.6399999999999</v>
+      </c>
+      <c r="AO17">
+        <f>U17-AB17-AC17-AD17</f>
+        <v>664</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" ref="AP17" si="16">100+0.2*(U17-100)</f>
+        <v>240</v>
+      </c>
+      <c r="AQ17" s="10"/>
     </row>
-    <row r="18" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AK18" s="25"/>
-      <c r="AO18" s="9"/>
-      <c r="AR18" s="9"/>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="I18" s="3">
+        <v>438</v>
+      </c>
+      <c r="J18" s="3">
+        <v>80</v>
+      </c>
+      <c r="K18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>388</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>2019</v>
+      </c>
+      <c r="AH18" s="1">
+        <f t="shared" ref="AH18:AH19" si="17">AI18+AE18</f>
+        <v>812</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>424</v>
+      </c>
+      <c r="AJ18" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AK18" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="AL18">
+        <f t="shared" ref="AL18:AL19" si="18">(1+AK18)*424+(245+302)</f>
+        <v>1123.6399999999999</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="15"/>
+        <v>518</v>
+      </c>
+      <c r="AN18" s="26">
+        <f t="shared" ref="AN18:AN19" si="19">AL18+AM18</f>
+        <v>1641.6399999999999</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" ref="AO18:AO19" si="20">U18-AB18-AC18-AD18</f>
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="9"/>
     </row>
-    <row r="19" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AK19" s="25"/>
-      <c r="AO19" s="9"/>
-      <c r="AR19" s="9"/>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <f>AG19-G19</f>
+        <v>2016</v>
+      </c>
+      <c r="I19" s="3">
+        <v>438</v>
+      </c>
+      <c r="J19" s="3">
+        <v>80</v>
+      </c>
+      <c r="K19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>388</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>2019</v>
+      </c>
+      <c r="AH19" s="1">
+        <f t="shared" si="17"/>
+        <v>812</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>424</v>
+      </c>
+      <c r="AJ19" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AK19" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" si="18"/>
+        <v>1123.6399999999999</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="15"/>
+        <v>518</v>
+      </c>
+      <c r="AN19" s="26">
+        <f t="shared" si="19"/>
+        <v>1641.6399999999999</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="9"/>
     </row>
-    <row r="20" spans="34:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AK20" s="25"/>
-      <c r="AO20" s="9"/>
-      <c r="AR20" s="9"/>
+      <c r="AN20" s="9"/>
+      <c r="AQ20" s="9"/>
     </row>
-    <row r="21" spans="34:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AK21" s="25"/>
-      <c r="AO21" s="9"/>
-      <c r="AR21" s="9"/>
+      <c r="AN21" s="9"/>
+      <c r="AQ21" s="9"/>
     </row>
-    <row r="22" spans="34:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AK22" s="25"/>
-      <c r="AO22" s="9"/>
-      <c r="AR22" s="9"/>
+      <c r="AN22" s="9"/>
+      <c r="AQ22" s="9"/>
     </row>
-    <row r="23" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO23" s="9"/>
-      <c r="AR23" s="9"/>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN23" s="9"/>
+      <c r="AQ23" s="9"/>
     </row>
-    <row r="24" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO24" s="9"/>
-      <c r="AR24" s="9"/>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN24" s="9"/>
+      <c r="AQ24" s="9"/>
     </row>
-    <row r="25" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO25" s="9"/>
-      <c r="AR25" s="9"/>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN25" s="9"/>
+      <c r="AQ25" s="9"/>
     </row>
-    <row r="26" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO26" s="9"/>
-      <c r="AR26" s="9"/>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN26" s="9"/>
+      <c r="AQ26" s="9"/>
     </row>
-    <row r="27" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO27" s="9"/>
-      <c r="AR27" s="9"/>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN27" s="9"/>
+      <c r="AQ27" s="9"/>
     </row>
-    <row r="28" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO28" s="9"/>
-      <c r="AR28" s="9"/>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN28" s="9"/>
+      <c r="AQ28" s="9"/>
     </row>
-    <row r="29" spans="34:44" x14ac:dyDescent="0.25">
-      <c r="AO29" s="9"/>
-      <c r="AR29" s="9"/>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN29" s="9"/>
+      <c r="AQ29" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ALG2 wealth test corrected
Former-commit-id: 2df0d6f28a5e1377630e46b7038364eacfb22273
Former-commit-id: d8944268b2b30e0cc61d1d943c18a0d143a0a3b6
</commit_message>
<xml_diff>
--- a/pre-waf/tests/test_data/test_dfs_alg2.xlsx
+++ b/pre-waf/tests/test_data/test_dfs_alg2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>hid</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>ar_alg2_ek_hh</t>
+  </si>
+  <si>
+    <t>vermfreibetr</t>
+  </si>
+  <si>
+    <t>maxvermfb</t>
   </si>
 </sst>
 </file>
@@ -543,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +690,12 @@
       <c r="AP1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="13"/>
+      <c r="AQ1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -710,7 +721,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H19" si="0">AG2-G2</f>
+        <f t="shared" ref="H2:H18" si="0">AG2-G2</f>
         <v>1986</v>
       </c>
       <c r="I2">
@@ -944,7 +955,7 @@
         <v>460</v>
       </c>
       <c r="AJ3" s="1">
-        <f t="shared" ref="AJ3:AJ19" si="7">$AO3-$AP3</f>
+        <f t="shared" ref="AJ3:AJ21" si="7">$AO3-$AP3</f>
         <v>0</v>
       </c>
       <c r="AK3">
@@ -2832,7 +2843,7 @@
       </c>
       <c r="AQ16" s="9"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2972,7 +2983,7 @@
       </c>
       <c r="AQ17" s="10"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>6</v>
       </c>
@@ -3108,7 +3119,7 @@
       </c>
       <c r="AQ18" s="9"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -3244,46 +3255,323 @@
       </c>
       <c r="AQ19" s="9"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AK20" s="25"/>
-      <c r="AN20" s="9"/>
-      <c r="AQ20" s="9"/>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>75</v>
+      </c>
+      <c r="H20" s="2">
+        <f>AG20-G20</f>
+        <v>1935</v>
+      </c>
+      <c r="I20" s="2">
+        <v>500</v>
+      </c>
+      <c r="J20" s="2">
+        <v>100</v>
+      </c>
+      <c r="K20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>2</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <v>0</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
+        <v>0</v>
+      </c>
+      <c r="W20" s="8">
+        <f>AF20/12</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="X20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="2">
+        <v>800</v>
+      </c>
+      <c r="AG20" s="2">
+        <v>2010</v>
+      </c>
+      <c r="AH20" s="1">
+        <f>AI20+AE20</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AI20" s="1">
+        <f>AJ20+AJ21</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AJ20" s="1">
+        <f>$AO20-$AP20</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <f>2*359*0.9</f>
+        <v>646.20000000000005</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" ref="AM20:AM21" si="21">I20+J20</f>
+        <v>600</v>
+      </c>
+      <c r="AN20" s="26">
+        <f>IF(AF20/0.025&gt;$AQ$20+$AQ$21,0,AL20+AM20)</f>
+        <v>1246.2</v>
+      </c>
+      <c r="AO20">
+        <f>W20+U20-AB20-AC20-AD20</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="9">
+        <f>MIN(MAX(3100,520*G20),AR20)</f>
+        <v>33800</v>
+      </c>
+      <c r="AR20">
+        <v>33800</v>
+      </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AK21" s="25"/>
-      <c r="AN21" s="9"/>
-      <c r="AQ21" s="9"/>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>50</v>
+      </c>
+      <c r="H21" s="3">
+        <f>AG21-G21</f>
+        <v>1960</v>
+      </c>
+      <c r="I21" s="3">
+        <v>500</v>
+      </c>
+      <c r="J21" s="3">
+        <v>100</v>
+      </c>
+      <c r="K21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>800</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>2010</v>
+      </c>
+      <c r="AH21" s="1">
+        <f t="shared" ref="AH20:AH21" si="22">AI21+AE21</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AI21" s="1">
+        <f>AJ21+AJ20</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AJ21" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <f>2*359*0.9</f>
+        <v>646.20000000000005</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="21"/>
+        <v>600</v>
+      </c>
+      <c r="AN21" s="26">
+        <f>IF(AF21/0.025&gt;$AQ$20+$AQ$21,0,AL21+AM21)</f>
+        <v>1246.2</v>
+      </c>
+      <c r="AO21">
+        <f>W21+U21-AB21-AC21-AD21</f>
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="9">
+        <f>MIN(MAX(3100,150*G21),AR21)</f>
+        <v>7500</v>
+      </c>
+      <c r="AR21">
+        <v>10050</v>
+      </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AK22" s="25"/>
       <c r="AN22" s="9"/>
       <c r="AQ22" s="9"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN23" s="9"/>
       <c r="AQ23" s="9"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN24" s="9"/>
       <c r="AQ24" s="9"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN25" s="9"/>
       <c r="AQ25" s="9"/>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN26" s="9"/>
       <c r="AQ26" s="9"/>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN27" s="9"/>
       <c r="AQ27" s="9"/>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN28" s="9"/>
       <c r="AQ28" s="9"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN29" s="9"/>
       <c r="AQ29" s="9"/>
     </row>

</xml_diff>

<commit_message>
UHV (Unterhaltsvorschuss) for single parents modelled and tested. some progress on UBI modelling
Former-commit-id: 723ac8081b4787ac6e6ca254a89b3f95ddb5d23b
Former-commit-id: 6176cebade064646df387d7fd0354b38f213715c
</commit_message>
<xml_diff>
--- a/pre-waf/tests/test_data/test_dfs_alg2.xlsx
+++ b/pre-waf/tests/test_data/test_dfs_alg2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>hid</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>maxvermfb</t>
+  </si>
+  <si>
+    <t>uhv</t>
   </si>
 </sst>
 </file>
@@ -547,23 +550,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU29"/>
+  <dimension ref="A1:AV29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI22" sqref="AI22"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="14" max="15" width="9.140625" customWidth="1"/>
-    <col min="34" max="34" width="15.7109375" customWidth="1"/>
-    <col min="38" max="38" width="12.5703125" customWidth="1"/>
-    <col min="39" max="39" width="14.7109375" customWidth="1"/>
-    <col min="40" max="40" width="16.140625" customWidth="1"/>
-    <col min="41" max="41" width="9.28515625" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" customWidth="1"/>
+    <col min="39" max="39" width="12.5703125" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" customWidth="1"/>
+    <col min="41" max="41" width="16.140625" customWidth="1"/>
+    <col min="42" max="42" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -658,46 +661,49 @@
         <v>31</v>
       </c>
       <c r="AF1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AH1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -721,7 +727,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H18" si="0">AG2-G2</f>
+        <f t="shared" ref="H2:H18" si="0">AH2-G2</f>
         <v>1986</v>
       </c>
       <c r="I2">
@@ -801,47 +807,50 @@
         <v>0</v>
       </c>
       <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
         <v>2016</v>
       </c>
-      <c r="AH2" s="12">
-        <f>AI2+AE2</f>
+      <c r="AI2" s="12">
+        <f>AJ2+AE2</f>
         <v>650</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AJ2" s="1">
         <v>460</v>
       </c>
-      <c r="AJ2" s="26">
-        <f>$AO2-$AP2</f>
+      <c r="AK2" s="26">
+        <f>$AP2-$AQ2</f>
         <v>400</v>
       </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
       <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
         <f>2*364+237</f>
         <v>965</v>
       </c>
-      <c r="AM2" s="9">
-        <f t="shared" ref="AM2:AM14" si="2">I2+J2</f>
+      <c r="AN2" s="9">
+        <f t="shared" ref="AN2:AN14" si="2">I2+J2</f>
         <v>800</v>
       </c>
-      <c r="AN2" s="26">
-        <f>AL2+AM2</f>
+      <c r="AO2" s="26">
+        <f>AM2+AN2</f>
         <v>1765</v>
       </c>
-      <c r="AO2" s="11">
+      <c r="AP2" s="11">
         <f>U2-AB2-AC2-AD2</f>
         <v>680</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <f>100+0.2*(U2-100)</f>
         <v>280</v>
       </c>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="5"/>
-      <c r="AU2" s="11"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="5"/>
+      <c r="AV2" s="11"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -945,46 +954,49 @@
         <v>0</v>
       </c>
       <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
         <v>2016</v>
       </c>
-      <c r="AH3" s="12">
-        <f t="shared" ref="AH3:AH13" si="6">AI3+AE3</f>
+      <c r="AI3" s="12">
+        <f t="shared" ref="AI3:AI13" si="6">AJ3+AE3</f>
         <v>650</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AJ3" s="1">
         <v>460</v>
       </c>
-      <c r="AJ3" s="1">
-        <f t="shared" ref="AJ3:AJ21" si="7">$AO3-$AP3</f>
-        <v>0</v>
-      </c>
-      <c r="AK3">
+      <c r="AK3" s="1">
+        <f t="shared" ref="AK3:AK21" si="7">$AP3-$AQ3</f>
         <v>0</v>
       </c>
       <c r="AL3">
-        <f t="shared" ref="AL3:AL4" si="8">2*364+237</f>
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" ref="AM3:AM4" si="8">2*364+237</f>
         <v>965</v>
       </c>
-      <c r="AM3" s="9">
+      <c r="AN3" s="9">
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="AN3" s="26">
-        <f t="shared" ref="AN3:AN16" si="9">AL3+AM3</f>
+      <c r="AO3" s="26">
+        <f t="shared" ref="AO3:AO16" si="9">AM3+AN3</f>
         <v>1765</v>
       </c>
-      <c r="AO3" s="11">
+      <c r="AP3" s="11">
         <f>U3-AB3-AC3-AD3</f>
         <v>0</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="9"/>
-      <c r="AR3" s="5"/>
-      <c r="AU3" s="11"/>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="5"/>
+      <c r="AV3" s="11"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1088,45 +1100,48 @@
         <v>0</v>
       </c>
       <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
         <v>2016</v>
       </c>
-      <c r="AH4" s="12">
+      <c r="AI4" s="12">
         <f t="shared" si="6"/>
         <v>650</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AJ4" s="1">
         <v>460</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AK4" s="1">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
       <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
         <f t="shared" si="8"/>
         <v>965</v>
       </c>
-      <c r="AM4" s="9">
+      <c r="AN4" s="9">
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
-      <c r="AN4" s="26">
+      <c r="AO4" s="26">
         <f t="shared" si="9"/>
         <v>1765</v>
       </c>
-      <c r="AO4" s="11">
+      <c r="AP4" s="11">
         <v>160</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>100</v>
       </c>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="5"/>
-      <c r="AU4" s="11"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="5"/>
+      <c r="AV4" s="11"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1229,49 +1244,52 @@
         <v>0</v>
       </c>
       <c r="AG5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2">
         <v>2013</v>
       </c>
-      <c r="AH5" s="23">
+      <c r="AI5" s="23">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
-      <c r="AI5" s="21">
+      <c r="AJ5" s="21">
         <v>500</v>
       </c>
-      <c r="AJ5" s="21">
+      <c r="AK5" s="21">
         <f t="shared" si="7"/>
         <v>500</v>
       </c>
-      <c r="AK5" s="2">
-        <v>0</v>
-      </c>
       <c r="AL5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AM5" s="10">
+      <c r="AN5" s="10">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN5" s="27">
+      <c r="AO5" s="27">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
-      <c r="AO5" s="15">
+      <c r="AP5" s="15">
         <f>U5+Y5-AB5-AC5-AD5</f>
         <v>740</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <f>100+0.2*(U5-100)</f>
         <v>240</v>
       </c>
-      <c r="AQ5" s="10"/>
-      <c r="AR5" s="8"/>
+      <c r="AR5" s="10"/>
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
-      <c r="AU5" s="11"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="11"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1374,48 +1392,51 @@
         <v>0</v>
       </c>
       <c r="AG6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
         <v>2013</v>
       </c>
-      <c r="AH6" s="24">
+      <c r="AI6" s="24">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
-      <c r="AI6" s="22">
+      <c r="AJ6" s="22">
         <v>500</v>
       </c>
-      <c r="AJ6" s="22">
+      <c r="AK6" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="2">
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="2">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AM6" s="9">
+      <c r="AN6" s="9">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN6" s="28">
+      <c r="AO6" s="28">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
-      <c r="AO6" s="19">
-        <f t="shared" ref="AO6:AO16" si="10">U6-AB6-AC6-AD6</f>
-        <v>0</v>
-      </c>
-      <c r="AP6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="20"/>
-      <c r="AR6" s="6"/>
+      <c r="AP6" s="19">
+        <f t="shared" ref="AP6:AP16" si="10">U6-AB6-AC6-AD6</f>
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="20"/>
       <c r="AS6" s="6"/>
       <c r="AT6" s="6"/>
-      <c r="AU6" s="11"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="11"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1518,50 +1539,53 @@
         <v>0</v>
       </c>
       <c r="AG7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="2">
         <v>2009</v>
       </c>
-      <c r="AH7" s="23">
-        <f>AI7+AE7</f>
+      <c r="AI7" s="23">
+        <f>AJ7+AE7</f>
         <v>848.5</v>
       </c>
-      <c r="AI7" s="21">
+      <c r="AJ7" s="21">
         <v>684.5</v>
       </c>
-      <c r="AJ7" s="21">
+      <c r="AK7" s="21">
         <f t="shared" si="7"/>
         <v>684.5</v>
       </c>
-      <c r="AK7" s="2">
+      <c r="AL7" s="2">
         <f>MAX(0.12*P7,0.36)</f>
         <v>0.36</v>
       </c>
-      <c r="AL7" s="2">
-        <f>(1+AK7)*359+(0.6*359)</f>
+      <c r="AM7" s="2">
+        <f>(1+AL7)*359+(0.6*359)</f>
         <v>703.64</v>
       </c>
-      <c r="AM7" s="10">
+      <c r="AN7" s="10">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN7" s="27">
+      <c r="AO7" s="27">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
-      <c r="AO7" s="15">
+      <c r="AP7" s="15">
         <f>U7+Y7-AB7-AC7-AD7</f>
         <v>944.5</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <f>100+0.2*(700)+0.1*200</f>
         <v>260</v>
       </c>
-      <c r="AQ7" s="10"/>
-      <c r="AR7" s="8"/>
+      <c r="AR7" s="10"/>
       <c r="AS7" s="8"/>
       <c r="AT7" s="8"/>
-      <c r="AU7" s="15"/>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="15"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1664,49 +1688,52 @@
         <v>0</v>
       </c>
       <c r="AG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
         <v>2009</v>
       </c>
-      <c r="AH8" s="24">
+      <c r="AI8" s="24">
         <f t="shared" si="6"/>
         <v>848.5</v>
       </c>
-      <c r="AI8" s="22">
+      <c r="AJ8" s="22">
         <v>684.5</v>
       </c>
-      <c r="AJ8" s="22">
+      <c r="AK8" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <f>MAX(0.12*P8,0.36)</f>
         <v>0.36</v>
       </c>
-      <c r="AL8" s="7">
-        <f>(1+AK8)*359+(0.6*359)</f>
+      <c r="AM8" s="7">
+        <f>(1+AL8)*359+(0.6*359)</f>
         <v>703.64</v>
       </c>
-      <c r="AM8" s="9">
+      <c r="AN8" s="9">
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-      <c r="AN8" s="29">
+      <c r="AO8" s="29">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
-      <c r="AO8" s="17">
+      <c r="AP8" s="17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="3"/>
+      <c r="AQ8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="9"/>
       <c r="AS8" s="3"/>
       <c r="AT8" s="3"/>
-      <c r="AU8" s="17"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="17"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1810,48 +1837,51 @@
         <v>0</v>
       </c>
       <c r="AG9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="2">
         <v>2006</v>
       </c>
-      <c r="AH9" s="23">
+      <c r="AI9" s="23">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AI9" s="21">
-        <v>0</v>
-      </c>
       <c r="AJ9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="21">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK9" s="2">
-        <v>0</v>
-      </c>
       <c r="AL9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="2">
         <f>345*0.9*2+345*0.6+345*0.7*2</f>
         <v>1311</v>
       </c>
-      <c r="AM9" s="10">
+      <c r="AN9" s="10">
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN9" s="27">
+      <c r="AO9" s="27">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AO9" s="15">
+      <c r="AP9" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" s="16"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="11"/>
+      <c r="AQ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="16"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="11"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1954,49 +1984,52 @@
       <c r="AF10" s="3">
         <v>0</v>
       </c>
-      <c r="AG10" s="4">
+      <c r="AG10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="4">
         <v>2006</v>
       </c>
-      <c r="AH10" s="12">
+      <c r="AI10" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AI10" s="22">
-        <v>0</v>
-      </c>
       <c r="AJ10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="3">
-        <f t="shared" ref="AL10:AL13" si="12">345*0.9*2+345*0.6+345*0.7*2</f>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="3">
+        <f t="shared" ref="AM10:AM13" si="12">345*0.9*2+345*0.6+345*0.7*2</f>
         <v>1311</v>
       </c>
-      <c r="AM10" s="9">
+      <c r="AN10" s="9">
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN10" s="29">
+      <c r="AO10" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AO10" s="17">
+      <c r="AP10" s="17">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="4"/>
-      <c r="AU10" s="11"/>
+      <c r="AQ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="18"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="11"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2099,48 +2132,51 @@
       <c r="AF11" s="3">
         <v>0</v>
       </c>
-      <c r="AG11" s="4">
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="4">
         <v>2006</v>
       </c>
-      <c r="AH11" s="12">
+      <c r="AI11" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AI11" s="22">
-        <v>0</v>
-      </c>
       <c r="AJ11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="3">
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="3">
         <f t="shared" si="12"/>
         <v>1311</v>
       </c>
-      <c r="AM11" s="9">
+      <c r="AN11" s="9">
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN11" s="29">
+      <c r="AO11" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AO11" s="11">
+      <c r="AP11" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="9"/>
-      <c r="AR11" s="5"/>
-      <c r="AS11" s="3"/>
-      <c r="AU11" s="11"/>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="3"/>
+      <c r="AV11" s="11"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2243,48 +2279,51 @@
       <c r="AF12" s="3">
         <v>0</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="4">
         <v>2006</v>
       </c>
-      <c r="AH12" s="12">
+      <c r="AI12" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AI12" s="22">
-        <v>0</v>
-      </c>
       <c r="AJ12" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK12" s="25">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="3">
+      <c r="AL12" s="25">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="3">
         <f t="shared" si="12"/>
         <v>1311</v>
       </c>
-      <c r="AM12" s="9">
+      <c r="AN12" s="9">
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN12" s="29">
+      <c r="AO12" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AO12" s="11">
+      <c r="AP12" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="5"/>
-      <c r="AS12" s="3"/>
-      <c r="AU12" s="11"/>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="3"/>
+      <c r="AV12" s="11"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2387,48 +2426,51 @@
       <c r="AF13" s="3">
         <v>0</v>
       </c>
-      <c r="AG13" s="4">
+      <c r="AG13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="4">
         <v>2006</v>
       </c>
-      <c r="AH13" s="12">
+      <c r="AI13" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AI13" s="22">
-        <v>0</v>
-      </c>
       <c r="AJ13" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK13" s="25">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="3">
+      <c r="AL13" s="25">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="3">
         <f t="shared" si="12"/>
         <v>1311</v>
       </c>
-      <c r="AM13" s="9">
+      <c r="AN13" s="9">
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-      <c r="AN13" s="29">
+      <c r="AO13" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
-      <c r="AO13" s="11">
+      <c r="AP13" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="5"/>
-      <c r="AS13" s="3"/>
-      <c r="AU13" s="11"/>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="3"/>
+      <c r="AV13" s="11"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2529,46 +2571,49 @@
         <v>0</v>
       </c>
       <c r="AG14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="2">
         <v>2011</v>
       </c>
-      <c r="AH14" s="21">
-        <f t="shared" ref="AH14:AH16" si="13">AI14+AE14</f>
+      <c r="AI14" s="21">
+        <f t="shared" ref="AI14:AI16" si="13">AJ14+AE14</f>
         <v>1289</v>
       </c>
-      <c r="AI14" s="21">
-        <f>AJ14+AJ16</f>
+      <c r="AJ14" s="21">
+        <f>AK14+AK16</f>
         <v>1289</v>
       </c>
-      <c r="AJ14" s="21">
+      <c r="AK14" s="21">
         <f t="shared" si="7"/>
         <v>849</v>
       </c>
-      <c r="AK14" s="8">
-        <v>0</v>
-      </c>
       <c r="AL14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AM14" s="2">
+      <c r="AN14" s="2">
         <f t="shared" si="2"/>
         <v>830</v>
       </c>
-      <c r="AN14" s="27">
+      <c r="AO14" s="27">
         <f t="shared" si="9"/>
         <v>1777</v>
       </c>
-      <c r="AO14" s="2">
+      <c r="AP14" s="2">
         <f t="shared" si="10"/>
         <v>1149</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <f>100+0.2*900+0.1*200</f>
         <v>300</v>
       </c>
-      <c r="AQ14" s="9"/>
+      <c r="AR14" s="9"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -2667,45 +2712,48 @@
       <c r="AF15" s="3">
         <v>0</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AG15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="2">
         <v>2011</v>
       </c>
-      <c r="AH15" s="1">
-        <f>AI15+AE15</f>
+      <c r="AI15" s="1">
+        <f>AJ15+AE15</f>
         <v>1289</v>
       </c>
-      <c r="AI15" s="1">
+      <c r="AJ15" s="1">
         <v>1289</v>
       </c>
-      <c r="AJ15" s="1">
+      <c r="AK15" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="8">
+      <c r="AL15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AM15">
-        <f t="shared" ref="AM15:AM16" si="14">I15+J15</f>
+      <c r="AN15">
+        <f t="shared" ref="AN15:AN16" si="14">I15+J15</f>
         <v>830</v>
       </c>
-      <c r="AN15" s="26">
+      <c r="AO15" s="26">
         <f t="shared" si="9"/>
         <v>1777</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="9"/>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="9"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -2804,46 +2852,49 @@
       <c r="AF16" s="3">
         <v>0</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AG16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="2">
         <v>2011</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AI16" s="1">
         <f t="shared" si="13"/>
         <v>1289</v>
       </c>
-      <c r="AI16" s="1">
+      <c r="AJ16" s="1">
         <v>1289</v>
       </c>
-      <c r="AJ16" s="1">
+      <c r="AK16" s="1">
         <f t="shared" si="7"/>
         <v>440</v>
       </c>
-      <c r="AK16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="8">
+      <c r="AL16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <f t="shared" si="14"/>
         <v>830</v>
       </c>
-      <c r="AN16" s="26">
+      <c r="AO16" s="26">
         <f t="shared" si="9"/>
         <v>1777</v>
       </c>
-      <c r="AO16">
+      <c r="AP16">
         <f t="shared" si="10"/>
         <v>680</v>
       </c>
-      <c r="AP16">
+      <c r="AQ16">
         <f>100+0.2*(U16-100)</f>
         <v>240</v>
       </c>
-      <c r="AQ16" s="9"/>
+      <c r="AR16" s="9"/>
     </row>
-    <row r="17" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2944,46 +2995,49 @@
         <v>0</v>
       </c>
       <c r="AG17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="2">
         <v>2019</v>
       </c>
-      <c r="AH17" s="1">
-        <f>AI17+AE17</f>
-        <v>812</v>
-      </c>
-      <c r="AI17" s="21">
-        <f>AJ17+AJ19</f>
+      <c r="AI17" s="1">
+        <f>AJ17+AE17+212+160</f>
+        <v>1184</v>
+      </c>
+      <c r="AJ17" s="21">
+        <f>AK17+AK19</f>
         <v>424</v>
       </c>
-      <c r="AJ17" s="1">
+      <c r="AK17" s="1">
         <f t="shared" si="7"/>
         <v>424</v>
       </c>
-      <c r="AK17" s="3">
+      <c r="AL17" s="3">
         <v>0.36</v>
       </c>
-      <c r="AL17">
-        <f>(1+AK17)*424+(245+302)</f>
+      <c r="AM17">
+        <f>(1+AL17)*424+(245+302)</f>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AM17">
-        <f t="shared" ref="AM17:AM19" si="15">I17+J17</f>
+      <c r="AN17">
+        <f t="shared" ref="AN17:AN19" si="15">I17+J17</f>
         <v>518</v>
       </c>
-      <c r="AN17" s="26">
-        <f>AL17+AM17</f>
+      <c r="AO17" s="26">
+        <f>AM17+AN17</f>
         <v>1641.6399999999999</v>
       </c>
-      <c r="AO17">
+      <c r="AP17">
         <f>U17-AB17-AC17-AD17</f>
         <v>664</v>
       </c>
-      <c r="AP17">
-        <f t="shared" ref="AP17" si="16">100+0.2*(U17-100)</f>
+      <c r="AQ17">
+        <f t="shared" ref="AQ17" si="16">100+0.2*(U17-100)</f>
         <v>240</v>
       </c>
-      <c r="AQ17" s="10"/>
+      <c r="AR17" s="10"/>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>6</v>
       </c>
@@ -3079,47 +3133,50 @@
         <v>388</v>
       </c>
       <c r="AF18" s="3">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="AG18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
         <v>2019</v>
       </c>
-      <c r="AH18" s="1">
-        <f t="shared" ref="AH18:AH19" si="17">AI18+AE18</f>
-        <v>812</v>
-      </c>
       <c r="AI18" s="1">
+        <f>AJ18+AE18+212+160</f>
+        <v>1184</v>
+      </c>
+      <c r="AJ18" s="1">
         <v>424</v>
       </c>
-      <c r="AJ18" s="1">
+      <c r="AK18" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK18" s="3">
+      <c r="AL18" s="3">
         <v>0.36</v>
       </c>
-      <c r="AL18">
-        <f t="shared" ref="AL18:AL19" si="18">(1+AK18)*424+(245+302)</f>
+      <c r="AM18">
+        <f t="shared" ref="AM18:AM19" si="17">(1+AL18)*424+(245+302)</f>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AM18">
+      <c r="AN18">
         <f t="shared" si="15"/>
         <v>518</v>
       </c>
-      <c r="AN18" s="26">
-        <f t="shared" ref="AN18:AN19" si="19">AL18+AM18</f>
+      <c r="AO18" s="26">
+        <f t="shared" ref="AO18:AO19" si="18">AM18+AN18</f>
         <v>1641.6399999999999</v>
       </c>
-      <c r="AO18">
-        <f t="shared" ref="AO18:AO19" si="20">U18-AB18-AC18-AD18</f>
-        <v>0</v>
-      </c>
       <c r="AP18">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="9"/>
+        <f t="shared" ref="AP18:AP19" si="19">U18-AB18-AC18-AD18</f>
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="9"/>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -3142,7 +3199,7 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <f>AG19-G19</f>
+        <f>AH19-G19</f>
         <v>2016</v>
       </c>
       <c r="I19" s="3">
@@ -3215,47 +3272,50 @@
         <v>388</v>
       </c>
       <c r="AF19" s="3">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AG19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
         <v>2019</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AI19" s="1">
+        <f>AJ19+AE19+212+160</f>
+        <v>1184</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>424</v>
+      </c>
+      <c r="AK19" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AL19" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="AM19">
         <f t="shared" si="17"/>
-        <v>812</v>
-      </c>
-      <c r="AI19" s="1">
-        <v>424</v>
-      </c>
-      <c r="AJ19" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AK19" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="AL19">
-        <f t="shared" si="18"/>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AM19">
+      <c r="AN19">
         <f t="shared" si="15"/>
         <v>518</v>
       </c>
-      <c r="AN19" s="26">
+      <c r="AO19" s="26">
+        <f t="shared" si="18"/>
+        <v>1641.6399999999999</v>
+      </c>
+      <c r="AP19">
         <f t="shared" si="19"/>
-        <v>1641.6399999999999</v>
-      </c>
-      <c r="AO19">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AP19">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="9"/>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -3278,7 +3338,7 @@
         <v>75</v>
       </c>
       <c r="H20" s="2">
-        <f>AG20-G20</f>
+        <f>AH20-G20</f>
         <v>1935</v>
       </c>
       <c r="I20" s="2">
@@ -3324,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="W20" s="8">
-        <f>AF20/12</f>
+        <f>AG20/12</f>
         <v>66.666666666666671</v>
       </c>
       <c r="X20" s="2">
@@ -3352,54 +3412,57 @@
         <v>0</v>
       </c>
       <c r="AF20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="2">
         <v>800</v>
       </c>
-      <c r="AG20" s="2">
+      <c r="AH20" s="2">
         <v>2010</v>
       </c>
-      <c r="AH20" s="1">
-        <f>AI20+AE20</f>
+      <c r="AI20" s="1">
+        <f>AJ20+AE20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AI20" s="1">
-        <f>AJ20+AJ21</f>
+      <c r="AJ20" s="1">
+        <f>AK20+AK21</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AJ20" s="1">
-        <f>$AO20-$AP20</f>
+      <c r="AK20" s="1">
+        <f>$AP20-$AQ20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AK20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL20">
+      <c r="AL20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM20">
         <f>2*359*0.9</f>
         <v>646.20000000000005</v>
       </c>
-      <c r="AM20">
-        <f t="shared" ref="AM20:AM21" si="21">I20+J20</f>
+      <c r="AN20">
+        <f t="shared" ref="AN20:AN21" si="20">I20+J20</f>
         <v>600</v>
       </c>
-      <c r="AN20" s="26">
-        <f>IF(AF20/0.025&gt;$AQ$20+$AQ$21,0,AL20+AM20)</f>
+      <c r="AO20" s="26">
+        <f>IF(AG20/0.025&gt;$AR$20+$AR$21,0,AM20+AN20)</f>
         <v>1246.2</v>
       </c>
-      <c r="AO20">
+      <c r="AP20">
         <f>W20+U20-AB20-AC20-AD20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AP20">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="9">
-        <f>MIN(MAX(3100,520*G20),AR20)</f>
+      <c r="AQ20">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="9">
+        <f>MIN(MAX(3100,520*G20),AS20)</f>
         <v>33800</v>
       </c>
-      <c r="AR20">
+      <c r="AS20">
         <v>33800</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>7</v>
       </c>
@@ -3422,7 +3485,7 @@
         <v>50</v>
       </c>
       <c r="H21" s="3">
-        <f>AG21-G21</f>
+        <f>AH21-G21</f>
         <v>1960</v>
       </c>
       <c r="I21" s="3">
@@ -3495,85 +3558,88 @@
         <v>0</v>
       </c>
       <c r="AF21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
         <v>800</v>
       </c>
-      <c r="AG21" s="3">
+      <c r="AH21" s="3">
         <v>2010</v>
       </c>
-      <c r="AH21" s="1">
-        <f t="shared" ref="AH20:AH21" si="22">AI21+AE21</f>
+      <c r="AI21" s="1">
+        <f t="shared" ref="AI21" si="21">AJ21+AE21</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AI21" s="1">
-        <f>AJ21+AJ20</f>
+      <c r="AJ21" s="1">
+        <f>AK21+AK20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AJ21" s="1">
+      <c r="AK21" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK21" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL21">
+      <c r="AL21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM21">
         <f>2*359*0.9</f>
         <v>646.20000000000005</v>
       </c>
-      <c r="AM21">
-        <f t="shared" si="21"/>
+      <c r="AN21">
+        <f t="shared" si="20"/>
         <v>600</v>
       </c>
-      <c r="AN21" s="26">
-        <f>IF(AF21/0.025&gt;$AQ$20+$AQ$21,0,AL21+AM21)</f>
+      <c r="AO21" s="26">
+        <f>IF(AG21/0.025&gt;$AR$20+$AR$21,0,AM21+AN21)</f>
         <v>1246.2</v>
       </c>
-      <c r="AO21">
+      <c r="AP21">
         <f>W21+U21-AB21-AC21-AD21</f>
         <v>0</v>
       </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-      <c r="AQ21" s="9">
-        <f>MIN(MAX(3100,150*G21),AR21)</f>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="9">
+        <f>MIN(MAX(3100,150*G21),AS21)</f>
         <v>7500</v>
       </c>
-      <c r="AR21">
+      <c r="AS21">
         <v>10050</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AK22" s="25"/>
-      <c r="AN22" s="9"/>
-      <c r="AQ22" s="9"/>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AL22" s="25"/>
+      <c r="AO22" s="9"/>
+      <c r="AR22" s="9"/>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN23" s="9"/>
-      <c r="AQ23" s="9"/>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO23" s="9"/>
+      <c r="AR23" s="9"/>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN24" s="9"/>
-      <c r="AQ24" s="9"/>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO24" s="9"/>
+      <c r="AR24" s="9"/>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN25" s="9"/>
-      <c r="AQ25" s="9"/>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO25" s="9"/>
+      <c r="AR25" s="9"/>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN26" s="9"/>
-      <c r="AQ26" s="9"/>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO26" s="9"/>
+      <c r="AR26" s="9"/>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN27" s="9"/>
-      <c r="AQ27" s="9"/>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO27" s="9"/>
+      <c r="AR27" s="9"/>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN28" s="9"/>
-      <c r="AQ28" s="9"/>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO28" s="9"/>
+      <c r="AR28" s="9"/>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AN29" s="9"/>
-      <c r="AQ29" s="9"/>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AO29" s="9"/>
+      <c r="AR29" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>